<commit_message>
Almost done. Help module still in progress (06-02-2022)
</commit_message>
<xml_diff>
--- a/Grade_Import/Evaluation Form_18-0000.xlsx
+++ b/Grade_Import/Evaluation Form_18-0000.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>EVALUATION FORM</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Curriculum Year:</t>
   </si>
   <si>
-    <t>Electrical Engineering</t>
+    <t>Civil Engineering</t>
   </si>
   <si>
     <t>Student Number:</t>
@@ -60,70 +60,58 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>EEO</t>
-  </si>
-  <si>
-    <t>Electrical Engineering Orientation</t>
+    <t>CE 24</t>
+  </si>
+  <si>
+    <t>CE Projec 2</t>
+  </si>
+  <si>
+    <t>CE 18</t>
+  </si>
+  <si>
+    <t>CE 25</t>
+  </si>
+  <si>
+    <t>Elective 3: Computer Software in Structural Analysis</t>
+  </si>
+  <si>
+    <t>CE 11 / CE 12</t>
+  </si>
+  <si>
+    <t>CE 26</t>
+  </si>
+  <si>
+    <t>Elective 4: Prestresssed Concrete Design</t>
+  </si>
+  <si>
+    <t>CE 12</t>
+  </si>
+  <si>
+    <t>CE 27</t>
+  </si>
+  <si>
+    <t>CE Elective 5</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>EM 1</t>
-  </si>
-  <si>
-    <t>Mathematics for Engineers 1</t>
-  </si>
-  <si>
-    <t>EM 2</t>
-  </si>
-  <si>
-    <t>Calculus 1 (Differential Calculus)</t>
-  </si>
-  <si>
-    <t>ES 1</t>
-  </si>
-  <si>
-    <t>Chemistry for Engineers with Lab</t>
-  </si>
-  <si>
-    <t>GE 2</t>
-  </si>
-  <si>
-    <t>Readings in Philippine History</t>
-  </si>
-  <si>
-    <t>GE 4</t>
-  </si>
-  <si>
-    <t>Mathematics in Modern World</t>
-  </si>
-  <si>
-    <t>GE 5</t>
-  </si>
-  <si>
-    <t>Purposive Communication</t>
-  </si>
-  <si>
-    <t>MST 1</t>
-  </si>
-  <si>
-    <t>Environmental Science</t>
-  </si>
-  <si>
-    <t>NSTP 1</t>
-  </si>
-  <si>
-    <t>National Training Service Program</t>
-  </si>
-  <si>
-    <t>PATHFIT 1</t>
-  </si>
-  <si>
-    <t>Physical Education 1</t>
-  </si>
-  <si>
-    <t>Test1 Student1</t>
+    <t>CE 28</t>
+  </si>
+  <si>
+    <t>CE Elective 6</t>
+  </si>
+  <si>
+    <t>CE 29</t>
+  </si>
+  <si>
+    <t>CE Integration Course 2</t>
+  </si>
+  <si>
+    <t>CE 23</t>
+  </si>
+  <si>
+    <t>Test Student1</t>
   </si>
   <si>
     <t>18-0000</t>
@@ -493,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G15"/>
+      <selection activeCell="G6" sqref="G6:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -525,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="5" t="s">
@@ -542,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="5" t="s">
@@ -579,7 +567,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -597,12 +585,12 @@
         <v>1.25</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
@@ -614,197 +602,105 @@
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F7" s="7">
         <v>1.5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F8" s="7">
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F9" s="7">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F10" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F11" s="7">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="1">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="7">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="7">
-        <v>2.25</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="7">
-        <v>1.75</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>